<commit_message>
Update result file for test_dofinance_parser_wrong_column_names
</commit_message>
<xml_diff>
--- a/tests/input/input_test_dofinance_parser_wrong_column_names.xlsx
+++ b/tests/input/input_test_dofinance_parser_wrong_column_names.xlsx
@@ -28,7 +28,7 @@
     <t xml:space="preserve">Bearbeitungsdatum</t>
   </si>
   <si>
-    <t xml:space="preserve">Art Transaktion</t>
+    <t xml:space="preserve">Dummy Column Name</t>
   </si>
   <si>
     <t xml:space="preserve">Investition ID</t>
@@ -485,7 +485,7 @@
   <dimension ref="A1:E491"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>